<commit_message>
Added template, models, queries for loans receivable, not yet tested
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/LOANS RECEIVABLE.xlsx
+++ b/aCCTg. pROGRAm/LOANS RECEIVABLE.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>LOANS RECEIVABLE</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>DONT FORGET TO DISPLAY CHARGE</t>
+  </si>
+  <si>
+    <t>Penalty Rate</t>
+  </si>
+  <si>
+    <t>Loan Amount</t>
   </si>
 </sst>
 </file>
@@ -287,6 +293,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,9 +308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -609,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,15 +661,15 @@
       <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
-      <c r="R3" s="8" t="s">
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="R3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="10"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -688,16 +694,16 @@
       <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="10"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="13"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3">
@@ -726,16 +732,16 @@
       <c r="J7" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="10"/>
+      <c r="N7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="13"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -752,17 +758,16 @@
       <c r="H9" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="S9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" s="9"/>
-      <c r="U9" s="10"/>
+      <c r="N9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="13"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -787,19 +792,17 @@
       <c r="H11" t="s">
         <v>41</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="N11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="11"/>
-      <c r="T11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" s="10"/>
+      <c r="S11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="12"/>
+      <c r="U11" s="13"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4">
@@ -815,6 +818,21 @@
         <v>42</v>
       </c>
     </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="13"/>
+      <c r="P13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="7"/>
+      <c r="T13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="13"/>
+    </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
@@ -833,6 +851,10 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
+      <c r="N15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -992,11 +1014,11 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
@@ -1090,16 +1112,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="N5:U5"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="S11:U11"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N9:U9"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:U7"/>
-    <mergeCell ref="T11:U11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>